<commit_message>
New AI project discussed with client
</commit_message>
<xml_diff>
--- a/Clients/AI Works.xlsx
+++ b/Clients/AI Works.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5. LIVE\AI ML PROJECTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\Clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C21675-4848-4102-88C1-8B4B5BA6A663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4223629C-B2D9-4025-9C2B-27B54624F5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Projects</t>
   </si>
@@ -113,13 +113,28 @@
   </si>
   <si>
     <t>Budget</t>
+  </si>
+  <si>
+    <t>Jotform usage and udpates to existing dashboard and flow</t>
+  </si>
+  <si>
+    <t>2023 - 02 - 28</t>
+  </si>
+  <si>
+    <t>Sr. #</t>
+  </si>
+  <si>
+    <t>GANs type of generative images for AI based eCommerce sites</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +187,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,29 +210,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -224,7 +253,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,112 +557,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="13">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>4</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>5</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>6</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="E10" s="19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="14">
-        <v>400</v>
-      </c>
+      <c r="F10" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -639,18 +759,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="2:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -661,13 +781,13 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>39</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -678,34 +798,34 @@
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>49</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="9" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+    <row r="6" spans="2:6" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+    <row r="7" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AI booth presentation sent to client + updates colab
</commit_message>
<xml_diff>
--- a/Clients/AI Works.xlsx
+++ b/Clients/AI Works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\Clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4223629C-B2D9-4025-9C2B-27B54624F5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102B5B85-9232-44A1-85B4-16F307DD621B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Projects</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Remarks</t>
-  </si>
-  <si>
-    <t>2023-02-09</t>
   </si>
   <si>
     <t>Meeting done</t>
@@ -128,19 +125,49 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Creating an async function in python that listens to order updates and accounts status for Alpaca trading</t>
+  </si>
+  <si>
+    <t>No meeting</t>
+  </si>
+  <si>
+    <t>zeg.ai</t>
+  </si>
+  <si>
+    <t>AI based photo booth for products</t>
+  </si>
+  <si>
+    <t>/ 5 photos</t>
+  </si>
+  <si>
+    <t>2023-03-02</t>
+  </si>
+  <si>
+    <t>booth.ai</t>
+  </si>
+  <si>
+    <t>AI based phototographer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -170,12 +197,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -190,6 +211,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -229,53 +257,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -573,166 +612,176 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="14">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="14">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
+        <v>6</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="14">
+        <v>7</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="D10" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="14">
         <v>8</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="13">
-        <v>2</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="D11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="13">
-        <v>3</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
-        <v>4</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
-        <v>5</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="20">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
-        <v>6</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
-        <v>7</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="F11" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -742,10 +791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879597FB-7C90-424A-87F6-FF2E07B75C03}">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -759,19 +808,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>7</v>
+      <c r="B2" s="25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
@@ -779,16 +828,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="9">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7">
         <v>39</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>20</v>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
@@ -796,36 +845,58 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="9">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7">
         <v>49</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="7">
+        <v>200</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Review of recommender system and TF-IDF system for new client
</commit_message>
<xml_diff>
--- a/Clients/AI Works.xlsx
+++ b/Clients/AI Works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\Clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102B5B85-9232-44A1-85B4-16F307DD621B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE171BB-5D94-4C26-A363-A02E42D856BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Projects</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Jotform usage and udpates to existing dashboard and flow</t>
   </si>
   <si>
-    <t>2023 - 02 - 28</t>
-  </si>
-  <si>
     <t>Sr. #</t>
   </si>
   <si>
@@ -149,13 +146,34 @@
   </si>
   <si>
     <t>AI based phototographer</t>
+  </si>
+  <si>
+    <t>Pre-process and create relation between data of an online community - Preprocess, vectorize, similarity, rank</t>
+  </si>
+  <si>
+    <t>Updated: 2023 - 02 - 28</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2023 - 01 - 17</t>
+  </si>
+  <si>
+    <t>2023 - 02 - 20</t>
+  </si>
+  <si>
+    <t>2023 - 03 - 02</t>
+  </si>
+  <si>
+    <t>2023 - 03 - 03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +236,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -257,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -315,6 +340,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B2:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -608,17 +642,19 @@
     <col min="2" max="2" width="7.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="63.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>0</v>
@@ -632,8 +668,11 @@
       <c r="F3" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G3" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>1</v>
       </c>
@@ -647,10 +686,14 @@
         <v>8</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>2</v>
       </c>
@@ -664,10 +707,13 @@
         <v>8</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>3</v>
       </c>
@@ -681,10 +727,13 @@
         <v>8</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <v>4</v>
       </c>
@@ -698,10 +747,13 @@
         <v>8</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -717,8 +769,11 @@
       <c r="F8" s="18">
         <v>400</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="G8" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="14">
         <v>6</v>
       </c>
@@ -732,15 +787,19 @@
         <v>8</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="2:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <v>7</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>7</v>
@@ -749,39 +808,62 @@
         <v>11</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="2:8" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B11" s="14">
         <v>8</v>
       </c>
       <c r="C11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>30</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" spans="2:8" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="14">
+        <v>9</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -793,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879597FB-7C90-424A-87F6-FF2E07B75C03}">
   <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -809,7 +891,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -873,16 +955,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="7">
         <v>200</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:6" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -890,10 +972,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="24"/>

</xml_diff>